<commit_message>
more file updates 4-18
</commit_message>
<xml_diff>
--- a/Task Schedule.xlsx
+++ b/Task Schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Embedded Systems\Security System Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Embedded Systems\Security System Project\BBBw-Security-System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A79860-3BF0-452C-B4A5-B1DF9C63217F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90617EB-2030-4C0E-BB38-B61051285237}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -352,7 +352,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -383,6 +383,18 @@
         <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -396,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -417,7 +429,6 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -443,6 +454,23 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -762,8 +790,8 @@
   </sheetPr>
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -776,7 +804,7 @@
     <col min="9" max="9" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -801,22 +829,22 @@
       <c r="K1" s="6"/>
     </row>
     <row r="2" spans="1:11" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+      <c r="A2" s="25">
         <v>1</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="26">
         <v>43571</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="27" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="9" t="s">
@@ -833,24 +861,24 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="174" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="12" t="s">
+      <c r="B3" s="30"/>
+      <c r="C3" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="31" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
@@ -860,7 +888,7 @@
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>19</v>
       </c>
@@ -871,38 +899,38 @@
       <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:11" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+      <c r="A6" s="25">
         <v>2</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="26">
         <v>43573</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="6" t="s">
+      <c r="C6" s="27"/>
+      <c r="D6" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="14"/>
+      <c r="F6" s="27"/>
     </row>
     <row r="7" spans="1:11" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="12" t="s">
+      <c r="B7" s="30"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="31" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>25</v>
       </c>
@@ -912,7 +940,7 @@
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>26</v>
       </c>
@@ -923,47 +951,47 @@
       <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:11" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="25">
         <v>3</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="26">
         <v>43573</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="24" t="s">
+      <c r="C10" s="27"/>
+      <c r="D10" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="E10" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="15"/>
+      <c r="F10" s="27"/>
     </row>
     <row r="11" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="12" t="s">
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="31" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
+    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
       <c r="B12" s="11"/>
       <c r="C12" s="13"/>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
+    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
       <c r="B13" s="11"/>
       <c r="C13" s="13"/>
       <c r="D13" s="12"/>
@@ -977,14 +1005,14 @@
       <c r="B14" s="8">
         <v>43578</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="23" t="s">
+      <c r="C14" s="14"/>
+      <c r="D14" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="15"/>
+      <c r="F14" s="14"/>
     </row>
     <row r="15" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
@@ -995,14 +1023,14 @@
       <c r="D15" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="24" t="s">
         <v>37</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>38</v>
       </c>
@@ -1011,11 +1039,11 @@
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+    </row>
+    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>39</v>
       </c>
@@ -1032,11 +1060,11 @@
       <c r="B18" s="8">
         <v>43580</v>
       </c>
-      <c r="C18" s="15"/>
+      <c r="C18" s="14"/>
       <c r="D18" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="23" t="s">
+      <c r="E18" s="22" t="s">
         <v>28</v>
       </c>
       <c r="F18" s="6" t="s">
@@ -1047,34 +1075,34 @@
       <c r="A19" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
       <c r="D19" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="25" t="s">
+      <c r="E19" s="24" t="s">
         <v>44</v>
       </c>
       <c r="F19" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
@@ -1086,28 +1114,28 @@
       <c r="B22" s="8">
         <v>43571</v>
       </c>
-      <c r="C22" s="15"/>
+      <c r="C22" s="14"/>
       <c r="D22" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E22" s="23" t="s">
+      <c r="E22" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="F22" s="15"/>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="12" t="s">
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="25" t="s">
+      <c r="E23" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="F23" s="31" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1115,26 +1143,26 @@
       <c r="A24" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
       <c r="D24" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="E24" s="25" t="s">
+      <c r="E24" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="F24" s="16"/>
+      <c r="F24" s="15"/>
     </row>
     <row r="25" spans="1:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
       <c r="D25" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="E25" s="25" t="s">
+      <c r="E25" s="24" t="s">
         <v>54</v>
       </c>
       <c r="F25" s="12" t="s">
@@ -1145,27 +1173,27 @@
       <c r="A26" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
       <c r="D26" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="E26" s="25" t="s">
+      <c r="E26" s="24" t="s">
         <v>57</v>
       </c>
       <c r="F26" s="12" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
-      <c r="F27" s="16"/>
+      <c r="F27" s="15"/>
     </row>
     <row r="28" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
@@ -1174,14 +1202,14 @@
       <c r="B28" s="8">
         <v>43580</v>
       </c>
-      <c r="C28" s="15"/>
+      <c r="C28" s="14"/>
       <c r="D28" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E28" s="23" t="s">
+      <c r="E28" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="F28" s="19" t="s">
+      <c r="F28" s="18" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1189,29 +1217,29 @@
       <c r="A29" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
       <c r="D29" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="E29" s="25" t="s">
+      <c r="E29" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="F29" s="20"/>
+      <c r="F29" s="19"/>
     </row>
     <row r="30" spans="1:6" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
       <c r="D30" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E30" s="25" t="s">
+      <c r="E30" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="F30" s="21">
+      <c r="F30" s="20">
         <v>5</v>
       </c>
     </row>
@@ -1222,57 +1250,57 @@
       <c r="B31" s="8">
         <v>43580</v>
       </c>
-      <c r="C31" s="15"/>
+      <c r="C31" s="14"/>
       <c r="D31" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E31" s="24" t="s">
+      <c r="E31" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="F31" s="22"/>
+      <c r="F31" s="21"/>
     </row>
     <row r="32" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B32" s="16"/>
-      <c r="C32" s="16"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
       <c r="D32" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="E32" s="25" t="s">
+      <c r="E32" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="F32" s="21">
+      <c r="F32" s="20">
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B33" s="16"/>
-      <c r="C33" s="16"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
-      <c r="F33" s="16"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F33" s="15"/>
+    </row>
+    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B34" s="16"/>
-      <c r="C34" s="16"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
       <c r="D34" s="12"/>
       <c r="E34" s="12"/>
-      <c r="F34" s="16"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F34" s="15"/>
+    </row>
+    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B35" s="16"/>
-      <c r="C35" s="16"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
       <c r="D35" s="12"/>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>

</xml_diff>